<commit_message>
Get data from excel
</commit_message>
<xml_diff>
--- a/ASCIWebApp/wwwroot/Հավելված 1.xlsx
+++ b/ASCIWebApp/wwwroot/Հավելված 1.xlsx
@@ -102,7 +102,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -110,6 +109,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,7 +395,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H5:H6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,144 +407,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>3425020293</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>3425020293</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>2470058141880000</v>
       </c>
-      <c r="D2" s="3">
-        <v>3425020293</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="D2" s="4">
+        <v>2470058141880000</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>3425020293</v>
-      </c>
-      <c r="B3" s="3">
-        <v>3425020293</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="A3" s="2">
+        <v>2356636565</v>
+      </c>
+      <c r="B3" s="2">
+        <v>5440014</v>
+      </c>
+      <c r="C3" s="2">
         <v>2470058141880000</v>
       </c>
-      <c r="D3" s="3">
-        <v>3425020293</v>
+      <c r="D3" s="2">
+        <v>2470058141880000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>